<commit_message>
modify code to functions
</commit_message>
<xml_diff>
--- a/groupSIFT_atlas.xlsx
+++ b/groupSIFT_atlas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\EEG_BCI\2. Word decoding\1. Temporal dynamic decoding\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\EEG_BCI\2. Word decoding\1. Temporal dynamic decoding\code\python\semantic_processing\graph_visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6120" windowHeight="12270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="for_circular_layout" sheetId="4" r:id="rId1"/>
@@ -304,18 +304,6 @@
     <t>Regions to be included</t>
   </si>
   <si>
-    <t>Upper_Basal_L</t>
-  </si>
-  <si>
-    <t>Upper_Basal_R</t>
-  </si>
-  <si>
-    <t>Lower_Basal_L</t>
-  </si>
-  <si>
-    <t>Lower_Basal_R</t>
-  </si>
-  <si>
     <t>Regions</t>
   </si>
   <si>
@@ -326,6 +314,18 @@
   </si>
   <si>
     <t>y_offset</t>
+  </si>
+  <si>
+    <t>UpperBasal_L</t>
+  </si>
+  <si>
+    <t>LowerBasal_L</t>
+  </si>
+  <si>
+    <t>LowerBasal_R</t>
+  </si>
+  <si>
+    <t>UpperBasal_R</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,16 +690,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B6" s="7">
         <v>6</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B34" s="7">
         <v>6</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B35" s="7">
         <v>6</v>
@@ -1776,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,22 +2152,22 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify offset for nodes labels
</commit_message>
<xml_diff>
--- a/groupSIFT_atlas.xlsx
+++ b/groupSIFT_atlas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="for_circular_layout" sheetId="4" r:id="rId1"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="6">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
         <v>-15</v>
       </c>
       <c r="D22" s="6">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>-20</v>
       </c>
       <c r="D23" s="6">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="6">
-        <v>-35</v>
+        <v>-30</v>
       </c>
       <c r="D24" s="6">
         <v>95</v>
@@ -1032,10 +1032,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="6">
-        <v>-45</v>
+        <v>-40</v>
       </c>
       <c r="D25" s="6">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,10 +1046,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="6">
-        <v>-50</v>
+        <v>-45</v>
       </c>
       <c r="D26" s="6">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>-55</v>
       </c>
       <c r="D27" s="6">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
         <v>-35</v>
       </c>
       <c r="D28" s="6">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,7 +1091,7 @@
         <v>-60</v>
       </c>
       <c r="D29" s="6">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="6">
-        <v>-70</v>
+        <v>-75</v>
       </c>
       <c r="D32" s="6">
         <v>50</v>
@@ -1147,7 +1147,7 @@
         <v>-45</v>
       </c>
       <c r="D33" s="6">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,10 +1158,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="6">
-        <v>-75</v>
+        <v>-70</v>
       </c>
       <c r="D34" s="6">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="6">
-        <v>-110</v>
+        <v>-115</v>
       </c>
       <c r="D36" s="6">
         <v>35</v>
@@ -1200,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="6">
-        <v>-110</v>
+        <v>-115</v>
       </c>
       <c r="D37" s="6">
         <v>25</v>
@@ -1214,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="6">
-        <v>-90</v>
+        <v>-95</v>
       </c>
       <c r="D38" s="6">
         <v>10</v>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="6">
-        <v>-90</v>
+        <v>-95</v>
       </c>
       <c r="D39" s="6">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="6">
-        <v>-85</v>
+        <v>-90</v>
       </c>
       <c r="D40" s="6">
         <v>-5</v>
@@ -1270,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="6">
-        <v>-85</v>
+        <v>-95</v>
       </c>
       <c r="D42" s="6">
         <v>-20</v>
@@ -1284,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="6">
-        <v>-60</v>
+        <v>-65</v>
       </c>
       <c r="D43" s="6">
         <v>-20</v>
@@ -1298,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="C44" s="6">
-        <v>-70</v>
+        <v>-75</v>
       </c>
       <c r="D44" s="6">
         <v>-30</v>
@@ -1312,7 +1312,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="6">
-        <v>-80</v>
+        <v>-85</v>
       </c>
       <c r="D45" s="6">
         <v>-45</v>
@@ -1326,7 +1326,7 @@
         <v>13</v>
       </c>
       <c r="C46" s="6">
-        <v>-50</v>
+        <v>-55</v>
       </c>
       <c r="D46" s="6">
         <v>-35</v>
@@ -1340,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="C47" s="6">
-        <v>-90</v>
+        <v>-95</v>
       </c>
       <c r="D47" s="6">
         <v>-70</v>
@@ -1354,10 +1354,10 @@
         <v>15</v>
       </c>
       <c r="C48" s="6">
-        <v>-40</v>
+        <v>-45</v>
       </c>
       <c r="D48" s="6">
-        <v>-40</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1368,10 +1368,10 @@
         <v>16</v>
       </c>
       <c r="C49" s="6">
-        <v>-60</v>
+        <v>-65</v>
       </c>
       <c r="D49" s="6">
-        <v>-65</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,10 +1410,10 @@
         <v>8</v>
       </c>
       <c r="C52" s="6">
-        <v>-45</v>
+        <v>-40</v>
       </c>
       <c r="D52" s="6">
-        <v>-70</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,10 +1424,10 @@
         <v>18</v>
       </c>
       <c r="C53" s="6">
-        <v>-25</v>
+        <v>-30</v>
       </c>
       <c r="D53" s="6">
-        <v>-60</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,10 +1438,10 @@
         <v>19</v>
       </c>
       <c r="C54" s="6">
-        <v>-35</v>
+        <v>-40</v>
       </c>
       <c r="D54" s="6">
-        <v>-90</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,10 +1466,10 @@
         <v>7</v>
       </c>
       <c r="C56" s="6">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="D56" s="6">
-        <v>-80</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,10 +1480,10 @@
         <v>7</v>
       </c>
       <c r="C57" s="6">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="D57" s="6">
-        <v>-80</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1497,7 +1497,7 @@
         <v>-5</v>
       </c>
       <c r="D58" s="6">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,8 +1510,8 @@
       <c r="C59" s="5">
         <v>-5</v>
       </c>
-      <c r="D59" s="5">
-        <v>-10</v>
+      <c r="D59" s="6">
+        <v>-15</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>-5</v>
       </c>
       <c r="D60" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1536,10 +1536,10 @@
         <v>7</v>
       </c>
       <c r="C61" s="5">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D61" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,10 +1550,10 @@
         <v>7</v>
       </c>
       <c r="C62" s="5">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D62" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,10 +1564,10 @@
         <v>19</v>
       </c>
       <c r="C63" s="5">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D63" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1592,10 +1592,10 @@
         <v>8</v>
       </c>
       <c r="C65" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D65" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,10 +1606,10 @@
         <v>8</v>
       </c>
       <c r="C66" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D66" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,10 +1620,10 @@
         <v>17</v>
       </c>
       <c r="C67" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D67" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,7 +1634,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D68" s="5">
         <v>-10</v>
@@ -1648,7 +1648,7 @@
         <v>15</v>
       </c>
       <c r="C69" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D69" s="5">
         <v>-10</v>
@@ -1662,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="C70" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D70" s="5">
         <v>-10</v>
@@ -1676,7 +1676,7 @@
         <v>13</v>
       </c>
       <c r="C71" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D71" s="5">
         <v>-10</v>
@@ -1690,7 +1690,7 @@
         <v>9</v>
       </c>
       <c r="C72" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D72" s="5">
         <v>-10</v>
@@ -1704,7 +1704,7 @@
         <v>12</v>
       </c>
       <c r="C73" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D73" s="5">
         <v>-10</v>
@@ -1718,7 +1718,7 @@
         <v>11</v>
       </c>
       <c r="C74" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D74" s="5">
         <v>-10</v>
@@ -1732,7 +1732,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D75" s="5">
         <v>-10</v>
@@ -1746,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D76" s="5">
         <v>-10</v>
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D77" s="5">
         <v>-10</v>
@@ -1776,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PLOT CONNECTION BETWEEN REGIONS LANGUAGE NETWORK, reference, 2017, Schoffelen, human brain for language
</commit_message>
<xml_diff>
--- a/groupSIFT_atlas.xlsx
+++ b/groupSIFT_atlas.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="12270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="for_circular_layout" sheetId="4" r:id="rId1"/>
-    <sheet name="Regions" sheetId="1" r:id="rId2"/>
-    <sheet name="Merged regions" sheetId="2" r:id="rId3"/>
+    <sheet name="language_network" sheetId="6" r:id="rId1"/>
+    <sheet name="for_circular_layout" sheetId="4" r:id="rId2"/>
+    <sheet name="Regions" sheetId="1" r:id="rId3"/>
+    <sheet name="Merged regions" sheetId="2" r:id="rId4"/>
+    <sheet name="language regions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
   <si>
     <t>'Hippocampus_L'</t>
   </si>
@@ -326,6 +328,147 @@
   </si>
   <si>
     <t>UpperBasal_R</t>
+  </si>
+  <si>
+    <t>AAL regions</t>
+  </si>
+  <si>
+    <t>BA09</t>
+  </si>
+  <si>
+    <t>BA17</t>
+  </si>
+  <si>
+    <t>BA18</t>
+  </si>
+  <si>
+    <t>BA19</t>
+  </si>
+  <si>
+    <t>BA46</t>
+  </si>
+  <si>
+    <t>BA44</t>
+  </si>
+  <si>
+    <t>BA45</t>
+  </si>
+  <si>
+    <t>BA47</t>
+  </si>
+  <si>
+    <t>BA06</t>
+  </si>
+  <si>
+    <t>BA39</t>
+  </si>
+  <si>
+    <t>BA40</t>
+  </si>
+  <si>
+    <t>sup.ant.temp</t>
+  </si>
+  <si>
+    <t>sup.middle.temp</t>
+  </si>
+  <si>
+    <t>sup.post.temp</t>
+  </si>
+  <si>
+    <t>middle.ant.temp</t>
+  </si>
+  <si>
+    <t>middle.middle.temp</t>
+  </si>
+  <si>
+    <t>middle.post.temp</t>
+  </si>
+  <si>
+    <t>inf.post.temp</t>
+  </si>
+  <si>
+    <t>Brodmann areas</t>
+  </si>
+  <si>
+    <t>Dorsolateral prefrontal cortex</t>
+  </si>
+  <si>
+    <t>Medial prefrontal cortex</t>
+  </si>
+  <si>
+    <t>Opercular part of inferior frontal gyrus</t>
+  </si>
+  <si>
+    <t>Ventro-lateral prefrontal cortex</t>
+  </si>
+  <si>
+    <t>Supplementary motor cortex</t>
+  </si>
+  <si>
+    <t>Angular gyrus</t>
+  </si>
+  <si>
+    <t>Intra-parietal sulcus</t>
+  </si>
+  <si>
+    <t>Cuneus</t>
+  </si>
+  <si>
+    <t>Secondary visual cortex</t>
+  </si>
+  <si>
+    <t>Primary visual cortex</t>
+  </si>
+  <si>
+    <t>superior anterior temporal</t>
+  </si>
+  <si>
+    <t>superior middle temporal</t>
+  </si>
+  <si>
+    <t>superior posterior temporal</t>
+  </si>
+  <si>
+    <t>middle anterior temporal</t>
+  </si>
+  <si>
+    <t>middle middle temporal</t>
+  </si>
+  <si>
+    <t>middle posterior temporal</t>
+  </si>
+  <si>
+    <t>inferior posterior temporal</t>
+  </si>
+  <si>
+    <t>Inferior frontal cortex</t>
+  </si>
+  <si>
+    <t>Name of Brodmann area</t>
+  </si>
+  <si>
+    <t>SFG, SFGO, MFG</t>
+  </si>
+  <si>
+    <t>SFGO, IFG</t>
+  </si>
+  <si>
+    <t>IFG, IFGO</t>
+  </si>
+  <si>
+    <t>PrC, RO</t>
+  </si>
+  <si>
+    <t>ITG,IPL, TPM</t>
+  </si>
+  <si>
+    <t>HES, STG, TPS, MTG, TPM, ITG</t>
+  </si>
+  <si>
+    <t>Q, ITG, MOG,FUSI,AG, SMG, IOG</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -381,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -391,6 +534,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,6 +561,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://journals.plos.org/plosone/article/figure/image?size=large&amp;id=10.1371/journal.pone.0196773.g002"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6772275" y="57150"/>
+          <a:ext cx="6334125" cy="7248525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,10 +878,939 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>-2</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="8">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="7">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="7">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2</v>
+      </c>
+      <c r="C22" s="6">
+        <v>-15</v>
+      </c>
+      <c r="D22" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-20</v>
+      </c>
+      <c r="D23" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-30</v>
+      </c>
+      <c r="D24" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-40</v>
+      </c>
+      <c r="D25" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="6">
+        <v>-45</v>
+      </c>
+      <c r="D26" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2</v>
+      </c>
+      <c r="C27" s="6">
+        <v>-55</v>
+      </c>
+      <c r="D27" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="7">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6">
+        <v>-60</v>
+      </c>
+      <c r="D29" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6">
+        <v>-75</v>
+      </c>
+      <c r="D30" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="7">
+        <v>3</v>
+      </c>
+      <c r="C31" s="6">
+        <v>-85</v>
+      </c>
+      <c r="D31" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="8">
+        <v>6</v>
+      </c>
+      <c r="C35" s="6">
+        <v>-75</v>
+      </c>
+      <c r="D35" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="8">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>-115</v>
+      </c>
+      <c r="D36" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>-115</v>
+      </c>
+      <c r="D37" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>-95</v>
+      </c>
+      <c r="D38" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6">
+        <v>-95</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6">
+        <v>-90</v>
+      </c>
+      <c r="D40" s="6">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="7">
+        <v>3</v>
+      </c>
+      <c r="C41" s="6">
+        <v>-75</v>
+      </c>
+      <c r="D41" s="6">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="7">
+        <v>11</v>
+      </c>
+      <c r="C43" s="6">
+        <v>-65</v>
+      </c>
+      <c r="D43" s="6">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="9">
+        <v>12</v>
+      </c>
+      <c r="C44" s="6">
+        <v>-75</v>
+      </c>
+      <c r="D44" s="6">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="7">
+        <v>9</v>
+      </c>
+      <c r="C45" s="6">
+        <v>-85</v>
+      </c>
+      <c r="D45" s="6">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="7">
+        <v>13</v>
+      </c>
+      <c r="C46" s="6">
+        <v>-55</v>
+      </c>
+      <c r="D46" s="6">
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="7">
+        <v>15</v>
+      </c>
+      <c r="C48" s="6">
+        <v>-45</v>
+      </c>
+      <c r="D48" s="6">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="7">
+        <v>8</v>
+      </c>
+      <c r="C51" s="6">
+        <v>-45</v>
+      </c>
+      <c r="D51" s="6">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" s="7">
+        <v>8</v>
+      </c>
+      <c r="C52" s="6">
+        <v>-40</v>
+      </c>
+      <c r="D52" s="6">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="7"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="7"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B55" s="7">
+        <v>7</v>
+      </c>
+      <c r="C55" s="6">
+        <v>-25</v>
+      </c>
+      <c r="D55" s="6">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="7">
+        <v>7</v>
+      </c>
+      <c r="C56" s="6">
+        <v>-20</v>
+      </c>
+      <c r="D56" s="6">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="7">
+        <v>7</v>
+      </c>
+      <c r="C57" s="6">
+        <v>-10</v>
+      </c>
+      <c r="D57" s="6">
+        <v>-95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="7">
+        <v>7</v>
+      </c>
+      <c r="C58" s="6">
+        <v>-5</v>
+      </c>
+      <c r="D58" s="6">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="7">
+        <v>7</v>
+      </c>
+      <c r="C59" s="5">
+        <v>-5</v>
+      </c>
+      <c r="D59" s="6">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="7">
+        <v>7</v>
+      </c>
+      <c r="C60" s="5">
+        <v>-5</v>
+      </c>
+      <c r="D60" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="7">
+        <v>7</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="7">
+        <v>7</v>
+      </c>
+      <c r="C62" s="5">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="7">
+        <v>8</v>
+      </c>
+      <c r="C65" s="5">
+        <v>5</v>
+      </c>
+      <c r="D65" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="7">
+        <v>8</v>
+      </c>
+      <c r="C66" s="5">
+        <v>5</v>
+      </c>
+      <c r="D66" s="5">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="7"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="7"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="7">
+        <v>15</v>
+      </c>
+      <c r="C69" s="5">
+        <v>10</v>
+      </c>
+      <c r="D69" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="7">
+        <v>13</v>
+      </c>
+      <c r="C71" s="5">
+        <v>10</v>
+      </c>
+      <c r="D71" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="7">
+        <v>9</v>
+      </c>
+      <c r="C72" s="5">
+        <v>10</v>
+      </c>
+      <c r="D72" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73" s="9">
+        <v>12</v>
+      </c>
+      <c r="C73" s="5">
+        <v>10</v>
+      </c>
+      <c r="D73" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="7">
+        <v>11</v>
+      </c>
+      <c r="C74" s="5">
+        <v>10</v>
+      </c>
+      <c r="D74" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="7"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" s="7">
+        <v>3</v>
+      </c>
+      <c r="C76" s="5">
+        <v>15</v>
+      </c>
+      <c r="D76" s="5">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77" s="7">
+        <v>1</v>
+      </c>
+      <c r="C77" s="5">
+        <v>15</v>
+      </c>
+      <c r="D77" s="5">
+        <v>-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K17:K19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>-5</v>
@@ -724,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>-5</v>
@@ -738,10 +1871,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>-5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,7 +1888,7 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -783,7 +1916,7 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,7 +1930,7 @@
         <v>15</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -811,7 +1944,7 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -825,7 +1958,7 @@
         <v>15</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -1634,10 +2767,10 @@
         <v>16</v>
       </c>
       <c r="C68" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D68" s="5">
-        <v>-10</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1732,7 +2865,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="5">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D75" s="5">
         <v>-10</v>
@@ -1746,7 +2879,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D76" s="5">
         <v>-10</v>
@@ -1760,10 +2893,10 @@
         <v>1</v>
       </c>
       <c r="C77" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D77" s="5">
-        <v>-10</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>
@@ -1772,11 +2905,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
@@ -2176,7 +3309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -2290,4 +3423,213 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C17:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change edge color and appearance
</commit_message>
<xml_diff>
--- a/groupSIFT_atlas.xlsx
+++ b/groupSIFT_atlas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\EEG_BCI\2. Word decoding\1. Temporal dynamic decoding\code\python\semantic_processing\graph_visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA78F16-88BF-4685-B9D4-0955061E7E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="language_network" sheetId="6" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="146">
   <si>
     <t>'Hippocampus_L'</t>
   </si>
@@ -304,9 +305,6 @@
   </si>
   <si>
     <t>Regions to be included</t>
-  </si>
-  <si>
-    <t>Regions</t>
   </si>
   <si>
     <t>color_index</t>
@@ -474,7 +472,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -524,25 +522,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,7 +571,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="https://journals.plos.org/plosone/article/figure/image?size=large&amp;id=10.1371/journal.pone.0196773.g002"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://journals.plos.org/plosone/article/figure/image?size=large&amp;id=10.1371/journal.pone.0196773.g002">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -877,969 +874,1165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" customWidth="1"/>
     <col min="10" max="10" width="36.140625" customWidth="1"/>
     <col min="11" max="11" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>146</v>
-      </c>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-2</v>
       </c>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="8">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="7">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>15</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5">
         <v>2</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
       <c r="D14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5">
         <v>2</v>
       </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
       <c r="D15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
       <c r="D16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
       <c r="D17">
         <v>10</v>
       </c>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="5">
         <v>2</v>
       </c>
-      <c r="C18">
-        <v>10</v>
-      </c>
       <c r="D18">
         <v>10</v>
       </c>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
       <c r="D19">
         <v>10</v>
       </c>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5">
         <v>2</v>
       </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
       <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5">
         <v>2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="D21" s="4">
         <v>0</v>
       </c>
-      <c r="D21" s="6">
+      <c r="E21" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="D22" s="4">
         <v>-15</v>
       </c>
-      <c r="D22" s="6">
+      <c r="E22" s="4">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="5">
         <v>2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="D23" s="4">
         <v>-20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="E23" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5">
         <v>2</v>
       </c>
-      <c r="C24" s="6">
+      <c r="D24" s="4">
         <v>-30</v>
       </c>
-      <c r="D24" s="6">
+      <c r="E24" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="5">
         <v>2</v>
       </c>
-      <c r="C25" s="6">
+      <c r="D25" s="4">
         <v>-40</v>
       </c>
-      <c r="D25" s="6">
+      <c r="E25" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="5">
         <v>2</v>
       </c>
-      <c r="C26" s="6">
+      <c r="D26" s="4">
         <v>-45</v>
       </c>
-      <c r="D26" s="6">
+      <c r="E26" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="C27" s="6">
+      <c r="D27" s="4">
         <v>-55</v>
       </c>
-      <c r="D27" s="6">
+      <c r="E27" s="4">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5">
         <v>2</v>
       </c>
-      <c r="C29" s="6">
+      <c r="D29" s="4">
         <v>-60</v>
       </c>
-      <c r="D29" s="6">
+      <c r="E29" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="5">
         <v>2</v>
       </c>
-      <c r="C30" s="6">
+      <c r="D30" s="4">
         <v>-75</v>
       </c>
-      <c r="D30" s="6">
+      <c r="E30" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="7">
-        <v>3</v>
-      </c>
-      <c r="C31" s="6">
-        <v>-85</v>
-      </c>
-      <c r="D31" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="8">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="5">
         <v>6</v>
       </c>
-      <c r="C35" s="6">
+      <c r="D35" s="4">
         <v>-75</v>
       </c>
-      <c r="D35" s="6">
+      <c r="E35" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="5">
         <v>1</v>
       </c>
-      <c r="C36" s="6">
+      <c r="D36" s="4">
         <v>-115</v>
       </c>
-      <c r="D36" s="6">
+      <c r="E36" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="5">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="D37" s="4">
         <v>-115</v>
       </c>
-      <c r="D37" s="6">
+      <c r="E37" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="5">
         <v>1</v>
       </c>
-      <c r="C38" s="6">
+      <c r="D38" s="4">
         <v>-95</v>
       </c>
-      <c r="D38" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="E38" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="5">
         <v>1</v>
       </c>
-      <c r="C39" s="6">
+      <c r="D39" s="4">
         <v>-95</v>
       </c>
-      <c r="D39" s="6">
+      <c r="E39" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="5">
         <v>1</v>
       </c>
-      <c r="C40" s="6">
+      <c r="D40" s="4">
         <v>-90</v>
       </c>
-      <c r="D40" s="6">
+      <c r="E40" s="4">
         <v>-5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="5">
         <v>3</v>
       </c>
-      <c r="C41" s="6">
+      <c r="D41" s="4">
         <v>-75</v>
       </c>
-      <c r="D41" s="6">
+      <c r="E41" s="4">
         <v>-10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="5">
         <v>11</v>
       </c>
-      <c r="C43" s="6">
+      <c r="D43" s="4">
         <v>-65</v>
       </c>
-      <c r="D43" s="6">
+      <c r="E43" s="4">
         <v>-20</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="5">
         <v>12</v>
       </c>
-      <c r="C44" s="6">
+      <c r="D44" s="4">
         <v>-75</v>
       </c>
-      <c r="D44" s="6">
+      <c r="E44" s="4">
         <v>-30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="5">
         <v>9</v>
       </c>
-      <c r="C45" s="6">
+      <c r="D45" s="4">
         <v>-85</v>
       </c>
-      <c r="D45" s="6">
+      <c r="E45" s="4">
         <v>-45</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="5">
         <v>13</v>
       </c>
-      <c r="C46" s="6">
+      <c r="D46" s="4">
         <v>-55</v>
       </c>
-      <c r="D46" s="6">
+      <c r="E46" s="4">
         <v>-35</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="5">
         <v>15</v>
       </c>
-      <c r="C48" s="6">
+      <c r="D48" s="4">
         <v>-45</v>
       </c>
-      <c r="D48" s="6">
+      <c r="E48" s="4">
         <v>-45</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="5">
         <v>8</v>
       </c>
-      <c r="C51" s="6">
+      <c r="D51" s="4">
         <v>-45</v>
       </c>
-      <c r="D51" s="6">
+      <c r="E51" s="4">
         <v>-65</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="5">
         <v>8</v>
       </c>
-      <c r="C52" s="6">
+      <c r="D52" s="4">
         <v>-40</v>
       </c>
-      <c r="D52" s="6">
+      <c r="E52" s="4">
         <v>-75</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="7"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="5">
         <v>7</v>
       </c>
-      <c r="C55" s="6">
+      <c r="D55" s="4">
         <v>-25</v>
       </c>
-      <c r="D55" s="6">
+      <c r="E55" s="4">
         <v>-80</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="5">
         <v>7</v>
       </c>
-      <c r="C56" s="6">
+      <c r="D56" s="4">
         <v>-20</v>
       </c>
-      <c r="D56" s="6">
+      <c r="E56" s="4">
         <v>-90</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="5">
         <v>7</v>
       </c>
-      <c r="C57" s="6">
+      <c r="D57" s="4">
         <v>-10</v>
       </c>
-      <c r="D57" s="6">
+      <c r="E57" s="4">
         <v>-95</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="5">
         <v>7</v>
       </c>
-      <c r="C58" s="6">
+      <c r="D58" s="4">
         <v>-5</v>
       </c>
-      <c r="D58" s="6">
+      <c r="E58" s="4">
         <v>-15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="5">
         <v>7</v>
       </c>
-      <c r="C59" s="5">
+      <c r="D59">
         <v>-5</v>
       </c>
-      <c r="D59" s="6">
+      <c r="E59" s="4">
         <v>-15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="5">
         <v>7</v>
       </c>
-      <c r="C60" s="5">
+      <c r="D60">
         <v>-5</v>
       </c>
-      <c r="D60" s="5">
+      <c r="E60">
         <v>-15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="5">
         <v>7</v>
       </c>
-      <c r="C61" s="5">
+      <c r="D61">
         <v>0</v>
       </c>
-      <c r="D61" s="5">
+      <c r="E61">
         <v>-15</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="5">
         <v>7</v>
       </c>
-      <c r="C62" s="5">
+      <c r="D62">
         <v>0</v>
       </c>
-      <c r="D62" s="5">
+      <c r="E62">
         <v>-15</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="7"/>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
       <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="5">
         <v>8</v>
       </c>
-      <c r="C65" s="5">
+      <c r="D65">
         <v>5</v>
       </c>
-      <c r="D65" s="5">
+      <c r="E65">
         <v>-15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="5">
         <v>8</v>
       </c>
-      <c r="C66" s="5">
+      <c r="D66">
         <v>5</v>
       </c>
-      <c r="D66" s="5">
+      <c r="E66">
         <v>-15</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="7"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="7"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>50</v>
+      </c>
       <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="5">
         <v>15</v>
       </c>
-      <c r="C69" s="5">
-        <v>10</v>
-      </c>
-      <c r="D69" s="5">
+      <c r="D69">
+        <v>10</v>
+      </c>
+      <c r="E69">
         <v>-10</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>80</v>
+      </c>
       <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="5">
         <v>13</v>
       </c>
-      <c r="C71" s="5">
-        <v>10</v>
-      </c>
-      <c r="D71" s="5">
+      <c r="D71">
+        <v>10</v>
+      </c>
+      <c r="E71">
         <v>-10</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="5">
         <v>9</v>
       </c>
-      <c r="C72" s="5">
-        <v>10</v>
-      </c>
-      <c r="D72" s="5">
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
         <v>-10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" s="5">
         <v>12</v>
       </c>
-      <c r="C73" s="5">
-        <v>10</v>
-      </c>
-      <c r="D73" s="5">
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73">
         <v>-10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" s="5">
         <v>11</v>
       </c>
-      <c r="C74" s="5">
-        <v>10</v>
-      </c>
-      <c r="D74" s="5">
+      <c r="D74">
+        <v>10</v>
+      </c>
+      <c r="E74">
         <v>-10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="7"/>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>36</v>
+      </c>
       <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="5">
         <v>3</v>
       </c>
-      <c r="C76" s="5">
+      <c r="D76">
         <v>15</v>
       </c>
-      <c r="D76" s="5">
+      <c r="E76">
         <v>-10</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" s="5">
         <v>1</v>
       </c>
-      <c r="C77" s="5">
+      <c r="D77">
         <v>15</v>
       </c>
-      <c r="D77" s="5">
+      <c r="E77">
         <v>-5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L17:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:D44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2">
@@ -1853,7 +2046,7 @@
       <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3">
@@ -1867,7 +2060,7 @@
       <c r="A4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4">
@@ -1881,7 +2074,7 @@
       <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5">
@@ -1893,9 +2086,9 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="7">
+        <v>97</v>
+      </c>
+      <c r="B6" s="5">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1907,9 +2100,9 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="7">
+        <v>98</v>
+      </c>
+      <c r="B7" s="5">
         <v>6</v>
       </c>
       <c r="C7">
@@ -1923,7 +2116,7 @@
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
       <c r="C8">
@@ -1937,7 +2130,7 @@
       <c r="A9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>4</v>
       </c>
       <c r="C9">
@@ -1951,7 +2144,7 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>3</v>
       </c>
       <c r="C10">
@@ -1965,7 +2158,7 @@
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11">
@@ -1979,7 +2172,7 @@
       <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12">
@@ -1993,7 +2186,7 @@
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>2</v>
       </c>
       <c r="C13">
@@ -2007,7 +2200,7 @@
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14">
@@ -2021,7 +2214,7 @@
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>2</v>
       </c>
       <c r="C15">
@@ -2035,7 +2228,7 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>2</v>
       </c>
       <c r="C16">
@@ -2049,7 +2242,7 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>2</v>
       </c>
       <c r="C17">
@@ -2063,7 +2256,7 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>2</v>
       </c>
       <c r="C18">
@@ -2077,7 +2270,7 @@
       <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>2</v>
       </c>
       <c r="C19">
@@ -2091,7 +2284,7 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>2</v>
       </c>
       <c r="C20">
@@ -2105,13 +2298,13 @@
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>2</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="4">
         <v>0</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="4">
         <v>85</v>
       </c>
     </row>
@@ -2119,13 +2312,13 @@
       <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <v>-15</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="4">
         <v>120</v>
       </c>
     </row>
@@ -2133,13 +2326,13 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>2</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="4">
         <v>-20</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>80</v>
       </c>
     </row>
@@ -2147,13 +2340,13 @@
       <c r="A24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>2</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>-30</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>95</v>
       </c>
     </row>
@@ -2161,13 +2354,13 @@
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>2</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>-40</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>95</v>
       </c>
     </row>
@@ -2175,13 +2368,13 @@
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>2</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>-45</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>95</v>
       </c>
     </row>
@@ -2189,13 +2382,13 @@
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>2</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>-55</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <v>90</v>
       </c>
     </row>
@@ -2203,13 +2396,13 @@
       <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>2</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>-35</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>45</v>
       </c>
     </row>
@@ -2217,13 +2410,13 @@
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>2</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="4">
         <v>-60</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>70</v>
       </c>
     </row>
@@ -2231,13 +2424,13 @@
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>2</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>-75</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>75</v>
       </c>
     </row>
@@ -2245,13 +2438,13 @@
       <c r="A31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>3</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <v>-85</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>70</v>
       </c>
     </row>
@@ -2259,13 +2452,13 @@
       <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="5">
         <v>4</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>-75</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>50</v>
       </c>
     </row>
@@ -2273,41 +2466,41 @@
       <c r="A33" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <v>5</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="4">
         <v>-45</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="7">
+        <v>95</v>
+      </c>
+      <c r="B34" s="5">
         <v>6</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>-70</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="7">
+        <v>96</v>
+      </c>
+      <c r="B35" s="5">
         <v>6</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="4">
         <v>-75</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <v>30</v>
       </c>
     </row>
@@ -2315,13 +2508,13 @@
       <c r="A36" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="5">
         <v>1</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="4">
         <v>-115</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="4">
         <v>35</v>
       </c>
     </row>
@@ -2329,13 +2522,13 @@
       <c r="A37" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="5">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="4">
         <v>-115</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="4">
         <v>25</v>
       </c>
     </row>
@@ -2343,13 +2536,13 @@
       <c r="A38" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="5">
         <v>1</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="4">
         <v>-95</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="4">
         <v>10</v>
       </c>
     </row>
@@ -2357,13 +2550,13 @@
       <c r="A39" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <v>1</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="4">
         <v>-95</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2371,13 +2564,13 @@
       <c r="A40" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="5">
         <v>1</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="4">
         <v>-90</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="4">
         <v>-5</v>
       </c>
     </row>
@@ -2385,13 +2578,13 @@
       <c r="A41" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="5">
         <v>3</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="4">
         <v>-75</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="4">
         <v>-10</v>
       </c>
     </row>
@@ -2399,13 +2592,13 @@
       <c r="A42" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="7">
-        <v>10</v>
-      </c>
-      <c r="C42" s="6">
+      <c r="B42" s="5">
+        <v>10</v>
+      </c>
+      <c r="C42" s="4">
         <v>-95</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="4">
         <v>-20</v>
       </c>
     </row>
@@ -2413,13 +2606,13 @@
       <c r="A43" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="5">
         <v>11</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="4">
         <v>-65</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>-20</v>
       </c>
     </row>
@@ -2427,13 +2620,13 @@
       <c r="A44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="5">
         <v>12</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="4">
         <v>-75</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="4">
         <v>-30</v>
       </c>
     </row>
@@ -2441,13 +2634,13 @@
       <c r="A45" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="5">
         <v>9</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="4">
         <v>-85</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="4">
         <v>-45</v>
       </c>
     </row>
@@ -2455,13 +2648,13 @@
       <c r="A46" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="5">
         <v>13</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="4">
         <v>-55</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <v>-35</v>
       </c>
     </row>
@@ -2469,13 +2662,13 @@
       <c r="A47" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="5">
         <v>14</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="4">
         <v>-95</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <v>-70</v>
       </c>
     </row>
@@ -2483,13 +2676,13 @@
       <c r="A48" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="5">
         <v>15</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="4">
         <v>-45</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <v>-45</v>
       </c>
     </row>
@@ -2497,13 +2690,13 @@
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="5">
         <v>16</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="4">
         <v>-65</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="4">
         <v>-70</v>
       </c>
     </row>
@@ -2511,13 +2704,13 @@
       <c r="A50" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="5">
         <v>17</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="4">
         <v>-50</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>-60</v>
       </c>
     </row>
@@ -2525,13 +2718,13 @@
       <c r="A51" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="5">
         <v>8</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="4">
         <v>-45</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="4">
         <v>-65</v>
       </c>
     </row>
@@ -2539,13 +2732,13 @@
       <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="5">
         <v>8</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="4">
         <v>-40</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="4">
         <v>-75</v>
       </c>
     </row>
@@ -2553,13 +2746,13 @@
       <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="5">
         <v>18</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53" s="4">
         <v>-30</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="4">
         <v>-65</v>
       </c>
     </row>
@@ -2567,13 +2760,13 @@
       <c r="A54" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="5">
         <v>19</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="4">
         <v>-40</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="4">
         <v>-95</v>
       </c>
     </row>
@@ -2581,13 +2774,13 @@
       <c r="A55" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="5">
         <v>7</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="4">
         <v>-25</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="4">
         <v>-80</v>
       </c>
     </row>
@@ -2595,13 +2788,13 @@
       <c r="A56" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="5">
         <v>7</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="4">
         <v>-20</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="4">
         <v>-90</v>
       </c>
     </row>
@@ -2609,13 +2802,13 @@
       <c r="A57" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="7">
+      <c r="B57" s="5">
         <v>7</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="4">
         <v>-10</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="4">
         <v>-95</v>
       </c>
     </row>
@@ -2623,13 +2816,13 @@
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="7">
+      <c r="B58" s="5">
         <v>7</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58" s="4">
         <v>-5</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="4">
         <v>-15</v>
       </c>
     </row>
@@ -2637,13 +2830,13 @@
       <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="5">
         <v>7</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59">
         <v>-5</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="4">
         <v>-15</v>
       </c>
     </row>
@@ -2651,13 +2844,13 @@
       <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="5">
         <v>7</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60">
         <v>-5</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D60">
         <v>-15</v>
       </c>
     </row>
@@ -2665,13 +2858,13 @@
       <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="5">
         <v>7</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61">
         <v>-15</v>
       </c>
     </row>
@@ -2679,13 +2872,13 @@
       <c r="A62" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="5">
         <v>7</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62">
         <v>0</v>
       </c>
-      <c r="D62" s="5">
+      <c r="D62">
         <v>-15</v>
       </c>
     </row>
@@ -2693,13 +2886,13 @@
       <c r="A63" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="7">
+      <c r="B63" s="5">
         <v>19</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63">
         <v>0</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D63">
         <v>-15</v>
       </c>
     </row>
@@ -2707,13 +2900,13 @@
       <c r="A64" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="7">
+      <c r="B64" s="5">
         <v>18</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D64">
         <v>-15</v>
       </c>
     </row>
@@ -2721,13 +2914,13 @@
       <c r="A65" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="7">
+      <c r="B65" s="5">
         <v>8</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65">
         <v>5</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65">
         <v>-15</v>
       </c>
     </row>
@@ -2735,13 +2928,13 @@
       <c r="A66" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="7">
+      <c r="B66" s="5">
         <v>8</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66">
         <v>5</v>
       </c>
-      <c r="D66" s="5">
+      <c r="D66">
         <v>-15</v>
       </c>
     </row>
@@ -2749,13 +2942,13 @@
       <c r="A67" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="7">
+      <c r="B67" s="5">
         <v>17</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67">
         <v>5</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D67">
         <v>-15</v>
       </c>
     </row>
@@ -2763,13 +2956,13 @@
       <c r="A68" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="5">
         <v>16</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68">
         <v>8</v>
       </c>
-      <c r="D68" s="5">
+      <c r="D68">
         <v>-15</v>
       </c>
     </row>
@@ -2777,13 +2970,13 @@
       <c r="A69" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="5">
         <v>15</v>
       </c>
-      <c r="C69" s="5">
-        <v>10</v>
-      </c>
-      <c r="D69" s="5">
+      <c r="C69">
+        <v>10</v>
+      </c>
+      <c r="D69">
         <v>-10</v>
       </c>
     </row>
@@ -2791,13 +2984,13 @@
       <c r="A70" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B70" s="5">
         <v>14</v>
       </c>
-      <c r="C70" s="5">
-        <v>10</v>
-      </c>
-      <c r="D70" s="5">
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
         <v>-10</v>
       </c>
     </row>
@@ -2805,13 +2998,13 @@
       <c r="A71" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="7">
+      <c r="B71" s="5">
         <v>13</v>
       </c>
-      <c r="C71" s="5">
-        <v>10</v>
-      </c>
-      <c r="D71" s="5">
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71">
         <v>-10</v>
       </c>
     </row>
@@ -2819,13 +3012,13 @@
       <c r="A72" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B72" s="5">
         <v>9</v>
       </c>
-      <c r="C72" s="5">
-        <v>10</v>
-      </c>
-      <c r="D72" s="5">
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
         <v>-10</v>
       </c>
     </row>
@@ -2833,13 +3026,13 @@
       <c r="A73" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="5">
         <v>12</v>
       </c>
-      <c r="C73" s="5">
-        <v>10</v>
-      </c>
-      <c r="D73" s="5">
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
         <v>-10</v>
       </c>
     </row>
@@ -2847,13 +3040,13 @@
       <c r="A74" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="5">
         <v>11</v>
       </c>
-      <c r="C74" s="5">
-        <v>10</v>
-      </c>
-      <c r="D74" s="5">
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74">
         <v>-10</v>
       </c>
     </row>
@@ -2861,13 +3054,13 @@
       <c r="A75" t="s">
         <v>36</v>
       </c>
-      <c r="B75" s="7">
-        <v>10</v>
-      </c>
-      <c r="C75" s="5">
+      <c r="B75" s="5">
+        <v>10</v>
+      </c>
+      <c r="C75">
         <v>13</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75">
         <v>-10</v>
       </c>
     </row>
@@ -2875,13 +3068,13 @@
       <c r="A76" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" s="5">
         <v>3</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76">
         <v>15</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76">
         <v>-10</v>
       </c>
     </row>
@@ -2889,13 +3082,13 @@
       <c r="A77" t="s">
         <v>90</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="5">
         <v>1</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77">
         <v>15</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77">
         <v>-5</v>
       </c>
     </row>
@@ -2906,7 +3099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3285,22 +3478,22 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3310,7 +3503,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3426,11 +3619,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,184 +3636,184 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>141</v>
+        <v>121</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="10"/>
+        <v>136</v>
+      </c>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="10"/>
+        <v>122</v>
+      </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>143</v>
+        <v>124</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="10"/>
+        <v>125</v>
+      </c>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>145</v>
+        <v>126</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C19" s="10"/>
+        <v>128</v>
+      </c>
+      <c r="C19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
add option to plot graph with or without node labels, change excel writing file to avoid overriding files with same name, add variable to indicate groupSIFT analysis scheme of choosing ICs, add abbreviation to regions in groupSIFT
</commit_message>
<xml_diff>
--- a/groupSIFT_atlas.xlsx
+++ b/groupSIFT_atlas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\EEG_BCI\2. Word decoding\1. Temporal dynamic decoding\code\python\semantic_processing\graph_visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA78F16-88BF-4685-B9D4-0955061E7E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EA803B-86FD-44E3-B4F5-001E5CBE2852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="266">
   <si>
     <t>'Hippocampus_L'</t>
   </si>
@@ -467,6 +467,366 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>MTG_R</t>
+  </si>
+  <si>
+    <t>MTG_L</t>
+  </si>
+  <si>
+    <t>STG_R</t>
+  </si>
+  <si>
+    <t>STG_L</t>
+  </si>
+  <si>
+    <t>ITG_L</t>
+  </si>
+  <si>
+    <t>MTP_R</t>
+  </si>
+  <si>
+    <t>STP_R</t>
+  </si>
+  <si>
+    <t>STP_L</t>
+  </si>
+  <si>
+    <t>MTP_L</t>
+  </si>
+  <si>
+    <t>LB_R</t>
+  </si>
+  <si>
+    <t>UB_R</t>
+  </si>
+  <si>
+    <t>UB_L</t>
+  </si>
+  <si>
+    <t>LB_L</t>
+  </si>
+  <si>
+    <t>C_L</t>
+  </si>
+  <si>
+    <t>C_R</t>
+  </si>
+  <si>
+    <t>In_R</t>
+  </si>
+  <si>
+    <t>In_L</t>
+  </si>
+  <si>
+    <t>ACing_R</t>
+  </si>
+  <si>
+    <t>SMA_R</t>
+  </si>
+  <si>
+    <t>IFOp_R</t>
+  </si>
+  <si>
+    <t>IFTri_R</t>
+  </si>
+  <si>
+    <t>Rec_R</t>
+  </si>
+  <si>
+    <t>SFOrb_R</t>
+  </si>
+  <si>
+    <t>MFOrb_R</t>
+  </si>
+  <si>
+    <t>IFOrb_R</t>
+  </si>
+  <si>
+    <t>SFMe_R</t>
+  </si>
+  <si>
+    <t>SFG_R</t>
+  </si>
+  <si>
+    <t>SFG_L</t>
+  </si>
+  <si>
+    <t>SFMed_L</t>
+  </si>
+  <si>
+    <t>IFOrb_L</t>
+  </si>
+  <si>
+    <t>MFOrb_L</t>
+  </si>
+  <si>
+    <t>SFOrb_L</t>
+  </si>
+  <si>
+    <t>IFTri_L</t>
+  </si>
+  <si>
+    <t>FMedOrb_R</t>
+  </si>
+  <si>
+    <t>FMedOrb_L</t>
+  </si>
+  <si>
+    <t>MFG_L</t>
+  </si>
+  <si>
+    <t>Rec_L</t>
+  </si>
+  <si>
+    <t>IFOp_L</t>
+  </si>
+  <si>
+    <t>SMA_L</t>
+  </si>
+  <si>
+    <t>ACing_L</t>
+  </si>
+  <si>
+    <t>PrC_L</t>
+  </si>
+  <si>
+    <t>RO_L</t>
+  </si>
+  <si>
+    <t>Fusi_L</t>
+  </si>
+  <si>
+    <t>PoC_L</t>
+  </si>
+  <si>
+    <t>SMG_L</t>
+  </si>
+  <si>
+    <t>AG_L</t>
+  </si>
+  <si>
+    <t>PCL_L</t>
+  </si>
+  <si>
+    <t>Ling_L</t>
+  </si>
+  <si>
+    <t>MCing_L</t>
+  </si>
+  <si>
+    <t>PQ_L</t>
+  </si>
+  <si>
+    <t>IPG_L</t>
+  </si>
+  <si>
+    <t>SPG_L</t>
+  </si>
+  <si>
+    <t>PCing_L</t>
+  </si>
+  <si>
+    <t>IOG_L</t>
+  </si>
+  <si>
+    <t>MOG_L</t>
+  </si>
+  <si>
+    <t>SOG_L</t>
+  </si>
+  <si>
+    <t>Q_L</t>
+  </si>
+  <si>
+    <t>Q_R</t>
+  </si>
+  <si>
+    <t>SOG_R</t>
+  </si>
+  <si>
+    <t>MOG_R</t>
+  </si>
+  <si>
+    <t>IOG_R</t>
+  </si>
+  <si>
+    <t>PCing_R</t>
+  </si>
+  <si>
+    <t>SPG_R</t>
+  </si>
+  <si>
+    <t>IPG_R</t>
+  </si>
+  <si>
+    <t>PQ_R</t>
+  </si>
+  <si>
+    <t>MCing_R</t>
+  </si>
+  <si>
+    <t>Ling_R</t>
+  </si>
+  <si>
+    <t>PCL_R</t>
+  </si>
+  <si>
+    <t>AG_R</t>
+  </si>
+  <si>
+    <t>SMG_R</t>
+  </si>
+  <si>
+    <t>PoC_R</t>
+  </si>
+  <si>
+    <t>Fusi_R</t>
+  </si>
+  <si>
+    <t>RO_R</t>
+  </si>
+  <si>
+    <t>PrC_R</t>
+  </si>
+  <si>
+    <t>ITF_R</t>
+  </si>
+  <si>
+    <t>abb</t>
+  </si>
+  <si>
+    <t>abb_1</t>
+  </si>
+  <si>
+    <t>MTG</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>STG</t>
+  </si>
+  <si>
+    <t>MTP</t>
+  </si>
+  <si>
+    <t>STP</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>ACing</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>IFOp</t>
+  </si>
+  <si>
+    <t>IFTri</t>
+  </si>
+  <si>
+    <t>Rec</t>
+  </si>
+  <si>
+    <t>FMedOrb</t>
+  </si>
+  <si>
+    <t>SFOrb</t>
+  </si>
+  <si>
+    <t>MFOrb</t>
+  </si>
+  <si>
+    <t>IFOrb</t>
+  </si>
+  <si>
+    <t>SFMe</t>
+  </si>
+  <si>
+    <t>SFG</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>SFMed</t>
+  </si>
+  <si>
+    <t>MFG</t>
+  </si>
+  <si>
+    <t>ITG</t>
+  </si>
+  <si>
+    <t>PrC</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>Fusi</t>
+  </si>
+  <si>
+    <t>PoC</t>
+  </si>
+  <si>
+    <t>SMG</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>PCL</t>
+  </si>
+  <si>
+    <t>Ling</t>
+  </si>
+  <si>
+    <t>MCing</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>IPG</t>
+  </si>
+  <si>
+    <t>SPG</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>PCing</t>
+  </si>
+  <si>
+    <t>IOG</t>
+  </si>
+  <si>
+    <t>MOG</t>
+  </si>
+  <si>
+    <t>SOG</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>ITF</t>
+  </si>
+  <si>
+    <t>hemisphere</t>
   </si>
 </sst>
 </file>
@@ -2000,1095 +2360,1791 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="5">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="5">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>-5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="5">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="5">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>15</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="5">
+      <c r="E6" s="5">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="5">
+      <c r="E7" s="5">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="F7">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="5">
+      <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="F8">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="5">
+      <c r="E9" s="5">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="5">
+      <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="F10">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5">
+      <c r="E11" s="5">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="F11">
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5">
+      <c r="E12" s="5">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="F12">
         <v>15</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="5">
+      <c r="E13" s="5">
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="F13">
         <v>15</v>
       </c>
-      <c r="D13">
+      <c r="G13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="5">
+      <c r="E14" s="5">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="F14">
         <v>10</v>
       </c>
-      <c r="D14">
+      <c r="G14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="5">
+      <c r="E15" s="5">
         <v>2</v>
       </c>
-      <c r="C15">
+      <c r="F15">
         <v>10</v>
       </c>
-      <c r="D15">
+      <c r="G15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5">
+      <c r="E16" s="5">
         <v>2</v>
       </c>
-      <c r="C16">
+      <c r="F16">
         <v>10</v>
       </c>
-      <c r="D16">
+      <c r="G16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5">
+      <c r="E17" s="5">
         <v>2</v>
       </c>
-      <c r="C17">
+      <c r="F17">
         <v>10</v>
       </c>
-      <c r="D17">
+      <c r="G17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="5">
+      <c r="E18" s="5">
         <v>2</v>
       </c>
-      <c r="C18">
+      <c r="F18">
         <v>10</v>
       </c>
-      <c r="D18">
+      <c r="G18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="5">
+      <c r="E19" s="5">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="F19">
         <v>10</v>
       </c>
-      <c r="D19">
+      <c r="G19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5">
+      <c r="E20" s="5">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="F20">
         <v>10</v>
       </c>
-      <c r="D20">
+      <c r="G20">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5">
+      <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="C21" s="4">
+      <c r="F21" s="4">
         <v>0</v>
       </c>
-      <c r="D21" s="4">
+      <c r="G21" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5">
+      <c r="E22" s="5">
         <v>2</v>
       </c>
-      <c r="C22" s="4">
+      <c r="F22" s="4">
         <v>-15</v>
       </c>
-      <c r="D22" s="4">
+      <c r="G22" s="4">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5">
+      <c r="E23" s="5">
         <v>2</v>
       </c>
-      <c r="C23" s="4">
+      <c r="F23" s="4">
         <v>-20</v>
       </c>
-      <c r="D23" s="4">
+      <c r="G23" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="5">
+      <c r="E24" s="5">
         <v>2</v>
       </c>
-      <c r="C24" s="4">
+      <c r="F24" s="4">
         <v>-30</v>
       </c>
-      <c r="D24" s="4">
+      <c r="G24" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="5">
+      <c r="E25" s="5">
         <v>2</v>
       </c>
-      <c r="C25" s="4">
+      <c r="F25" s="4">
         <v>-40</v>
       </c>
-      <c r="D25" s="4">
+      <c r="G25" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" t="s">
+        <v>237</v>
+      </c>
+      <c r="C26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="5">
+      <c r="E26" s="5">
         <v>2</v>
       </c>
-      <c r="C26" s="4">
+      <c r="F26" s="4">
         <v>-45</v>
       </c>
-      <c r="D26" s="4">
+      <c r="G26" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="5">
+      <c r="E27" s="5">
         <v>2</v>
       </c>
-      <c r="C27" s="4">
+      <c r="F27" s="4">
         <v>-55</v>
       </c>
-      <c r="D27" s="4">
+      <c r="G27" s="4">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="5">
+      <c r="E28" s="5">
         <v>2</v>
       </c>
-      <c r="C28" s="4">
+      <c r="F28" s="4">
         <v>-35</v>
       </c>
-      <c r="D28" s="4">
+      <c r="G28" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" t="s">
+        <v>242</v>
+      </c>
+      <c r="D29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="5">
+      <c r="E29" s="5">
         <v>2</v>
       </c>
-      <c r="C29" s="4">
+      <c r="F29" s="4">
         <v>-60</v>
       </c>
-      <c r="D29" s="4">
+      <c r="G29" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" t="s">
+        <v>233</v>
+      </c>
+      <c r="C30" t="s">
+        <v>242</v>
+      </c>
+      <c r="D30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="5">
+      <c r="E30" s="5">
         <v>2</v>
       </c>
-      <c r="C30" s="4">
+      <c r="F30" s="4">
         <v>-75</v>
       </c>
-      <c r="D30" s="4">
+      <c r="G30" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" t="s">
+        <v>242</v>
+      </c>
+      <c r="D31" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="5">
+      <c r="E31" s="5">
         <v>3</v>
       </c>
-      <c r="C31" s="4">
+      <c r="F31" s="4">
         <v>-85</v>
       </c>
-      <c r="D31" s="4">
+      <c r="G31" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" t="s">
+        <v>231</v>
+      </c>
+      <c r="C32" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="5">
+      <c r="E32" s="5">
         <v>4</v>
       </c>
-      <c r="C32" s="4">
+      <c r="F32" s="4">
         <v>-75</v>
       </c>
-      <c r="D32" s="4">
+      <c r="G32" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" t="s">
+        <v>230</v>
+      </c>
+      <c r="C33" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="5">
+      <c r="E33" s="5">
         <v>5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="F33" s="4">
         <v>-45</v>
       </c>
-      <c r="D33" s="4">
+      <c r="G33" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D34" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="5">
+      <c r="E34" s="5">
         <v>6</v>
       </c>
-      <c r="C34" s="4">
+      <c r="F34" s="4">
         <v>-70</v>
       </c>
-      <c r="D34" s="4">
+      <c r="G34" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="5">
+      <c r="E35" s="5">
         <v>6</v>
       </c>
-      <c r="C35" s="4">
+      <c r="F35" s="4">
         <v>-75</v>
       </c>
-      <c r="D35" s="4">
+      <c r="G35" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
+        <v>242</v>
+      </c>
+      <c r="D36" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="5">
+      <c r="E36" s="5">
         <v>1</v>
       </c>
-      <c r="C36" s="4">
+      <c r="F36" s="4">
         <v>-115</v>
       </c>
-      <c r="D36" s="4">
+      <c r="G36" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>226</v>
+      </c>
+      <c r="C37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D37" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="5">
+      <c r="E37" s="5">
         <v>1</v>
       </c>
-      <c r="C37" s="4">
+      <c r="F37" s="4">
         <v>-115</v>
       </c>
-      <c r="D37" s="4">
+      <c r="G37" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C38" t="s">
+        <v>242</v>
+      </c>
+      <c r="D38" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="5">
+      <c r="E38" s="5">
         <v>1</v>
       </c>
-      <c r="C38" s="4">
+      <c r="F38" s="4">
         <v>-95</v>
       </c>
-      <c r="D38" s="4">
+      <c r="G38" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="5">
+      <c r="E39" s="5">
         <v>1</v>
       </c>
-      <c r="C39" s="4">
+      <c r="F39" s="4">
         <v>-95</v>
       </c>
-      <c r="D39" s="4">
+      <c r="G39" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" t="s">
+        <v>245</v>
+      </c>
+      <c r="C40" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="5">
+      <c r="E40" s="5">
         <v>1</v>
       </c>
-      <c r="C40" s="4">
+      <c r="F40" s="4">
         <v>-90</v>
       </c>
-      <c r="D40" s="4">
+      <c r="G40" s="4">
         <v>-5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D41" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="5">
+      <c r="E41" s="5">
         <v>3</v>
       </c>
-      <c r="C41" s="4">
+      <c r="F41" s="4">
         <v>-75</v>
       </c>
-      <c r="D41" s="4">
+      <c r="G41" s="4">
         <v>-10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" t="s">
+        <v>247</v>
+      </c>
+      <c r="C42" t="s">
+        <v>242</v>
+      </c>
+      <c r="D42" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="5">
+      <c r="E42" s="5">
         <v>10</v>
       </c>
-      <c r="C42" s="4">
+      <c r="F42" s="4">
         <v>-95</v>
       </c>
-      <c r="D42" s="4">
+      <c r="G42" s="4">
         <v>-20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" t="s">
+        <v>242</v>
+      </c>
+      <c r="D43" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="5">
+      <c r="E43" s="5">
         <v>11</v>
       </c>
-      <c r="C43" s="4">
+      <c r="F43" s="4">
         <v>-65</v>
       </c>
-      <c r="D43" s="4">
+      <c r="G43" s="4">
         <v>-20</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" t="s">
+        <v>249</v>
+      </c>
+      <c r="C44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D44" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="5">
+      <c r="E44" s="5">
         <v>12</v>
       </c>
-      <c r="C44" s="4">
+      <c r="F44" s="4">
         <v>-75</v>
       </c>
-      <c r="D44" s="4">
+      <c r="G44" s="4">
         <v>-30</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" t="s">
+        <v>250</v>
+      </c>
+      <c r="C45" t="s">
+        <v>242</v>
+      </c>
+      <c r="D45" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5">
+      <c r="E45" s="5">
         <v>9</v>
       </c>
-      <c r="C45" s="4">
+      <c r="F45" s="4">
         <v>-85</v>
       </c>
-      <c r="D45" s="4">
+      <c r="G45" s="4">
         <v>-45</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" t="s">
+        <v>251</v>
+      </c>
+      <c r="C46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D46" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="5">
+      <c r="E46" s="5">
         <v>13</v>
       </c>
-      <c r="C46" s="4">
+      <c r="F46" s="4">
         <v>-55</v>
       </c>
-      <c r="D46" s="4">
+      <c r="G46" s="4">
         <v>-35</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" t="s">
+        <v>252</v>
+      </c>
+      <c r="C47" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="5">
+      <c r="E47" s="5">
         <v>14</v>
       </c>
-      <c r="C47" s="4">
+      <c r="F47" s="4">
         <v>-95</v>
       </c>
-      <c r="D47" s="4">
+      <c r="G47" s="4">
         <v>-70</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" t="s">
+        <v>253</v>
+      </c>
+      <c r="C48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="5">
+      <c r="E48" s="5">
         <v>15</v>
       </c>
-      <c r="C48" s="4">
+      <c r="F48" s="4">
         <v>-45</v>
       </c>
-      <c r="D48" s="4">
+      <c r="G48" s="4">
         <v>-45</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>194</v>
+      </c>
+      <c r="B49" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" t="s">
+        <v>242</v>
+      </c>
+      <c r="D49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="5">
+      <c r="E49" s="5">
         <v>16</v>
       </c>
-      <c r="C49" s="4">
+      <c r="F49" s="4">
         <v>-65</v>
       </c>
-      <c r="D49" s="4">
+      <c r="G49" s="4">
         <v>-70</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C50" t="s">
+        <v>242</v>
+      </c>
+      <c r="D50" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="5">
+      <c r="E50" s="5">
         <v>17</v>
       </c>
-      <c r="C50" s="4">
+      <c r="F50" s="4">
         <v>-50</v>
       </c>
-      <c r="D50" s="4">
+      <c r="G50" s="4">
         <v>-60</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
+        <v>256</v>
+      </c>
+      <c r="C51" t="s">
+        <v>242</v>
+      </c>
+      <c r="D51" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="5">
+      <c r="E51" s="5">
         <v>8</v>
       </c>
-      <c r="C51" s="4">
+      <c r="F51" s="4">
         <v>-45</v>
       </c>
-      <c r="D51" s="4">
+      <c r="G51" s="4">
         <v>-65</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" t="s">
+        <v>257</v>
+      </c>
+      <c r="C52" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="5">
+      <c r="E52" s="5">
         <v>8</v>
       </c>
-      <c r="C52" s="4">
+      <c r="F52" s="4">
         <v>-40</v>
       </c>
-      <c r="D52" s="4">
+      <c r="G52" s="4">
         <v>-75</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" t="s">
+        <v>242</v>
+      </c>
+      <c r="D53" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="5">
+      <c r="E53" s="5">
         <v>18</v>
       </c>
-      <c r="C53" s="4">
+      <c r="F53" s="4">
         <v>-30</v>
       </c>
-      <c r="D53" s="4">
+      <c r="G53" s="4">
         <v>-65</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" t="s">
+        <v>259</v>
+      </c>
+      <c r="C54" t="s">
+        <v>242</v>
+      </c>
+      <c r="D54" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="5">
+      <c r="E54" s="5">
         <v>19</v>
       </c>
-      <c r="C54" s="4">
+      <c r="F54" s="4">
         <v>-40</v>
       </c>
-      <c r="D54" s="4">
+      <c r="G54" s="4">
         <v>-95</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" t="s">
+        <v>260</v>
+      </c>
+      <c r="C55" t="s">
+        <v>242</v>
+      </c>
+      <c r="D55" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="5">
+      <c r="E55" s="5">
         <v>7</v>
       </c>
-      <c r="C55" s="4">
+      <c r="F55" s="4">
         <v>-25</v>
       </c>
-      <c r="D55" s="4">
+      <c r="G55" s="4">
         <v>-80</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" t="s">
+        <v>261</v>
+      </c>
+      <c r="C56" t="s">
+        <v>242</v>
+      </c>
+      <c r="D56" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="5">
+      <c r="E56" s="5">
         <v>7</v>
       </c>
-      <c r="C56" s="4">
+      <c r="F56" s="4">
         <v>-20</v>
       </c>
-      <c r="D56" s="4">
+      <c r="G56" s="4">
         <v>-90</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" t="s">
+        <v>242</v>
+      </c>
+      <c r="D57" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="5">
+      <c r="E57" s="5">
         <v>7</v>
       </c>
-      <c r="C57" s="4">
+      <c r="F57" s="4">
         <v>-10</v>
       </c>
-      <c r="D57" s="4">
+      <c r="G57" s="4">
         <v>-95</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B58" t="s">
+        <v>263</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="5">
+      <c r="E58" s="5">
         <v>7</v>
       </c>
-      <c r="C58" s="4">
+      <c r="F58" s="4">
         <v>-5</v>
       </c>
-      <c r="D58" s="4">
+      <c r="G58" s="4">
         <v>-15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>203</v>
+      </c>
+      <c r="B59" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" t="s">
+        <v>224</v>
+      </c>
+      <c r="D59" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="5">
+      <c r="E59" s="5">
         <v>7</v>
       </c>
-      <c r="C59">
+      <c r="F59">
         <v>-5</v>
       </c>
-      <c r="D59" s="4">
+      <c r="G59" s="4">
         <v>-15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="5">
+      <c r="E60" s="5">
         <v>7</v>
       </c>
-      <c r="C60">
+      <c r="F60">
         <v>-5</v>
       </c>
-      <c r="D60">
+      <c r="G60">
         <v>-15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" t="s">
+        <v>261</v>
+      </c>
+      <c r="C61" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="5">
+      <c r="E61" s="5">
         <v>7</v>
       </c>
-      <c r="C61">
+      <c r="F61">
         <v>0</v>
       </c>
-      <c r="D61">
+      <c r="G61">
         <v>-15</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" t="s">
+        <v>260</v>
+      </c>
+      <c r="C62" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" t="s">
         <v>64</v>
       </c>
-      <c r="B62" s="5">
+      <c r="E62" s="5">
         <v>7</v>
       </c>
-      <c r="C62">
+      <c r="F62">
         <v>0</v>
       </c>
-      <c r="D62">
+      <c r="G62">
         <v>-15</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" t="s">
+        <v>259</v>
+      </c>
+      <c r="C63" t="s">
+        <v>224</v>
+      </c>
+      <c r="D63" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="5">
+      <c r="E63" s="5">
         <v>19</v>
       </c>
-      <c r="C63">
+      <c r="F63">
         <v>0</v>
       </c>
-      <c r="D63">
+      <c r="G63">
         <v>-15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" t="s">
+        <v>224</v>
+      </c>
+      <c r="D64" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="5">
+      <c r="E64" s="5">
         <v>18</v>
       </c>
-      <c r="C64">
+      <c r="F64">
         <v>0</v>
       </c>
-      <c r="D64">
+      <c r="G64">
         <v>-15</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="5">
+      <c r="E65" s="5">
         <v>8</v>
       </c>
-      <c r="C65">
+      <c r="F65">
         <v>5</v>
       </c>
-      <c r="D65">
+      <c r="G65">
         <v>-15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" t="s">
+        <v>224</v>
+      </c>
+      <c r="D66" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="5">
+      <c r="E66" s="5">
         <v>8</v>
       </c>
-      <c r="C66">
+      <c r="F66">
         <v>5</v>
       </c>
-      <c r="D66">
+      <c r="G66">
         <v>-15</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>210</v>
+      </c>
+      <c r="B67" t="s">
+        <v>255</v>
+      </c>
+      <c r="C67" t="s">
+        <v>224</v>
+      </c>
+      <c r="D67" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="5">
+      <c r="E67" s="5">
         <v>17</v>
       </c>
-      <c r="C67">
+      <c r="F67">
         <v>5</v>
       </c>
-      <c r="D67">
+      <c r="G67">
         <v>-15</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>211</v>
+      </c>
+      <c r="B68" t="s">
+        <v>254</v>
+      </c>
+      <c r="C68" t="s">
+        <v>224</v>
+      </c>
+      <c r="D68" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="5">
+      <c r="E68" s="5">
         <v>16</v>
       </c>
-      <c r="C68">
+      <c r="F68">
         <v>8</v>
       </c>
-      <c r="D68">
+      <c r="G68">
         <v>-15</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C69" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="5">
+      <c r="E69" s="5">
         <v>15</v>
       </c>
-      <c r="C69">
+      <c r="F69">
         <v>10</v>
       </c>
-      <c r="D69">
+      <c r="G69">
         <v>-10</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B70" t="s">
+        <v>252</v>
+      </c>
+      <c r="C70" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="5">
+      <c r="E70" s="5">
         <v>14</v>
       </c>
-      <c r="C70">
+      <c r="F70">
         <v>10</v>
       </c>
-      <c r="D70">
+      <c r="G70">
         <v>-10</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" t="s">
+        <v>251</v>
+      </c>
+      <c r="C71" t="s">
+        <v>224</v>
+      </c>
+      <c r="D71" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="5">
+      <c r="E71" s="5">
         <v>13</v>
       </c>
-      <c r="C71">
+      <c r="F71">
         <v>10</v>
       </c>
-      <c r="D71">
+      <c r="G71">
         <v>-10</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>215</v>
+      </c>
+      <c r="B72" t="s">
+        <v>250</v>
+      </c>
+      <c r="C72" t="s">
+        <v>224</v>
+      </c>
+      <c r="D72" t="s">
         <v>74</v>
       </c>
-      <c r="B72" s="5">
+      <c r="E72" s="5">
         <v>9</v>
       </c>
-      <c r="C72">
+      <c r="F72">
         <v>10</v>
       </c>
-      <c r="D72">
+      <c r="G72">
         <v>-10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" t="s">
+        <v>224</v>
+      </c>
+      <c r="D73" t="s">
         <v>68</v>
       </c>
-      <c r="B73" s="5">
+      <c r="E73" s="5">
         <v>12</v>
       </c>
-      <c r="C73">
+      <c r="F73">
         <v>10</v>
       </c>
-      <c r="D73">
+      <c r="G73">
         <v>-10</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>217</v>
+      </c>
+      <c r="B74" t="s">
+        <v>248</v>
+      </c>
+      <c r="C74" t="s">
+        <v>224</v>
+      </c>
+      <c r="D74" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="5">
+      <c r="E74" s="5">
         <v>11</v>
       </c>
-      <c r="C74">
+      <c r="F74">
         <v>10</v>
       </c>
-      <c r="D74">
+      <c r="G74">
         <v>-10</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" t="s">
+        <v>247</v>
+      </c>
+      <c r="C75" t="s">
+        <v>224</v>
+      </c>
+      <c r="D75" t="s">
         <v>36</v>
       </c>
-      <c r="B75" s="5">
+      <c r="E75" s="5">
         <v>10</v>
       </c>
-      <c r="C75">
+      <c r="F75">
         <v>13</v>
       </c>
-      <c r="D75">
+      <c r="G75">
         <v>-10</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" t="s">
+        <v>246</v>
+      </c>
+      <c r="C76" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="5">
+      <c r="E76" s="5">
         <v>3</v>
       </c>
-      <c r="C76">
+      <c r="F76">
         <v>15</v>
       </c>
-      <c r="D76">
+      <c r="G76">
         <v>-10</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>220</v>
+      </c>
+      <c r="B77" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" t="s">
+        <v>224</v>
+      </c>
+      <c r="D77" t="s">
         <v>90</v>
       </c>
-      <c r="B77" s="5">
+      <c r="E77" s="5">
         <v>1</v>
       </c>
-      <c r="C77">
+      <c r="F77">
         <v>15</v>
       </c>
-      <c r="D77">
+      <c r="G77">
         <v>-5</v>
       </c>
     </row>

</xml_diff>